<commit_message>
[master] finished laravel assignment 2
</commit_message>
<xml_diff>
--- a/tutorials/review_points_nandaroo.xlsx
+++ b/tutorials/review_points_nandaroo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\php_training\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>№</t>
     <phoneticPr fontId="0"/>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Tutorial_05 index.php</t>
+  </si>
+  <si>
+    <t>laravel quick start login logout</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -312,11 +315,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -333,6 +356,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -342,18 +419,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -369,56 +440,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,7 +495,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8E36CC0-E148-4A4A-A479-E2B59189ABAE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E36CC0-E148-4A4A-A479-E2B59189ABAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -818,6 +856,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>283743</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1257300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5210175" y="7048500"/>
+          <a:ext cx="3103143" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1133,72 +1215,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="24"/>
-    <col min="2" max="2" width="10.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="9.140625" style="24"/>
-    <col min="15" max="15" width="16.28515625" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="9.140625" style="14"/>
+    <col min="2" max="2" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="14"/>
+    <col min="15" max="15" width="16.28515625" style="14" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="19" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:43" s="10" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="12" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="9" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="18" t="s">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="19" customFormat="1" ht="92.25" customHeight="1">
+    <row r="2" spans="1:43" s="10" customFormat="1" ht="92.25" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1214,31 +1296,31 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="26"/>
       <c r="O2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-    </row>
-    <row r="3" spans="1:25" s="19" customFormat="1" ht="75" customHeight="1">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+    </row>
+    <row r="3" spans="1:43" s="10" customFormat="1" ht="75" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1254,18 +1336,18 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="26" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="15" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="27"/>
@@ -1274,175 +1356,265 @@
       <c r="S3" s="27"/>
       <c r="T3" s="27"/>
       <c r="U3" s="27"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-    </row>
-    <row r="4" spans="1:25" ht="78" customHeight="1">
-      <c r="A4" s="22">
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+    </row>
+    <row r="4" spans="1:43" ht="78" customHeight="1">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="13">
         <v>44547</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="26" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-    </row>
-    <row r="5" spans="1:25" ht="88.5" customHeight="1">
-      <c r="A5" s="22">
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="39"/>
+    </row>
+    <row r="5" spans="1:43" ht="88.5" customHeight="1">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="13">
         <v>44547</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="26" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="22"/>
-    </row>
-    <row r="6" spans="1:25" ht="84" customHeight="1">
-      <c r="A6" s="29">
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="39"/>
+    </row>
+    <row r="6" spans="1:43" ht="84" customHeight="1">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="18">
         <v>44548</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="26" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-    </row>
-    <row r="7" spans="1:25" s="22" customFormat="1" ht="93.75" customHeight="1">
-      <c r="A7" s="22">
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="39"/>
+      <c r="AP6" s="39"/>
+      <c r="AQ6" s="39"/>
+    </row>
+    <row r="7" spans="1:43" s="12" customFormat="1" ht="93.75" customHeight="1">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="13">
         <v>44548</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
       <c r="O7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="19">
         <f ca="1">P7:U7</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="W7" s="37"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="39"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="39"/>
+      <c r="AE7" s="39"/>
+      <c r="AF7" s="39"/>
+      <c r="AG7" s="39"/>
+      <c r="AH7" s="39"/>
+      <c r="AI7" s="39"/>
+      <c r="AJ7" s="39"/>
+      <c r="AK7" s="39"/>
+      <c r="AL7" s="39"/>
+      <c r="AM7" s="39"/>
+      <c r="AN7" s="39"/>
+      <c r="AO7" s="39"/>
+      <c r="AP7" s="39"/>
+      <c r="AQ7" s="39"/>
+    </row>
+    <row r="8" spans="1:43" ht="114" customHeight="1">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>44560</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="P5:U5"/>
     <mergeCell ref="P6:U6"/>
@@ -1455,15 +1627,6 @@
     <mergeCell ref="I4:N4"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="I6:N6"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="P2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>